<commit_message>
Site updated: 2024-10-07 23:52:07
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -729,31 +729,31 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Site updated: 2024-10-09 08:24:45
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -766,13 +766,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -784,13 +784,13 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Site updated: 2024-10-09 09:00:21
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Site updated: 2024-10-10 23:51:13
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -840,31 +840,31 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">

</xml_diff>

<commit_message>
Site updated: 2024-10-11 23:53:34
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -877,31 +877,31 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
Site updated: 2024-10-12 23:49:49
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -914,19 +914,19 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
Site updated: 2024-10-14 07:35:55
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -951,31 +951,31 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
Site updated: 2024-10-14 23:47:54
</commit_message>
<xml_diff>
--- a/statistics/2024_Oct_principle_data.xlsx
+++ b/statistics/2024_Oct_principle_data.xlsx
@@ -988,31 +988,31 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">

</xml_diff>